<commit_message>
Adding the nse and ip validation
</commit_message>
<xml_diff>
--- a/files/rangeOfIPAddresses.xlsx
+++ b/files/rangeOfIPAddresses.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\poshan\tldr\tldr_fail_testing\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atish\Desktop\Programming\TLDR Fail\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EDE9F9E-2621-4045-A912-4E46812B12CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6007B6B-B080-4B7B-A9A3-DE2096123A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{EECDF66F-84CF-47E0-9AA0-E9C9E9760CBF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{EECDF66F-84CF-47E0-9AA0-E9C9E9760CBF}"/>
   </bookViews>
   <sheets>
     <sheet name="ipAddresses" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="1087">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="1088">
   <si>
     <t>102.112.0.0</t>
   </si>
@@ -3300,6 +3300,9 @@
   </si>
   <si>
     <t>Count</t>
+  </si>
+  <si>
+    <t>Total IP</t>
   </si>
 </sst>
 </file>
@@ -3682,18 +3685,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0677CDAD-B304-45E8-80F1-C56675B70DA3}">
-  <dimension ref="A1:C543"/>
+  <dimension ref="A1:D543"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="310" zoomScaleNormal="310" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.06640625" style="5"/>
+    <col min="3" max="3" width="9" style="5"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1084</v>
       </c>
@@ -3703,8 +3707,11 @@
       <c r="C1" s="5" t="s">
         <v>1086</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D1" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3714,8 +3721,12 @@
       <c r="C2" s="3">
         <v>524288</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D2" s="5">
+        <f xml:space="preserve"> SUM(C2:C543)</f>
+        <v>6482688</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -3726,7 +3737,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -3737,7 +3748,7 @@
         <v>2560</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -3748,7 +3759,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -3759,7 +3770,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -3770,7 +3781,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -3781,7 +3792,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -3792,7 +3803,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -3803,7 +3814,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -3814,7 +3825,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -3825,7 +3836,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -3836,7 +3847,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -3847,7 +3858,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
@@ -3858,7 +3869,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -3869,7 +3880,7 @@
         <v>3072</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>30</v>
       </c>
@@ -3880,7 +3891,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
@@ -3891,7 +3902,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>34</v>
       </c>
@@ -3902,7 +3913,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -3913,7 +3924,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>38</v>
       </c>
@@ -3924,7 +3935,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
@@ -3935,7 +3946,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>42</v>
       </c>
@@ -3946,7 +3957,7 @@
         <v>211200</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>44</v>
       </c>
@@ -3957,7 +3968,7 @@
         <v>50688</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>46</v>
       </c>
@@ -3968,7 +3979,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>48</v>
       </c>
@@ -3979,7 +3990,7 @@
         <v>7424</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>50</v>
       </c>
@@ -3990,7 +4001,7 @@
         <v>14336</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>52</v>
       </c>
@@ -4001,7 +4012,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>54</v>
       </c>
@@ -4012,7 +4023,7 @@
         <v>3072</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>56</v>
       </c>
@@ -4023,7 +4034,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>58</v>
       </c>
@@ -4034,7 +4045,7 @@
         <v>65536</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
@@ -4045,7 +4056,7 @@
         <v>1196032</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>62</v>
       </c>
@@ -4056,7 +4067,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>64</v>
       </c>
@@ -4067,7 +4078,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>66</v>
       </c>
@@ -4078,7 +4089,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>68</v>
       </c>
@@ -4089,7 +4100,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>70</v>
       </c>
@@ -4100,7 +4111,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>72</v>
       </c>
@@ -4111,7 +4122,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>74</v>
       </c>
@@ -4122,7 +4133,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>76</v>
       </c>
@@ -4133,7 +4144,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>78</v>
       </c>
@@ -4144,7 +4155,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>80</v>
       </c>
@@ -4155,7 +4166,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>82</v>
       </c>
@@ -4166,7 +4177,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>84</v>
       </c>
@@ -4177,7 +4188,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>86</v>
       </c>
@@ -4188,7 +4199,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>88</v>
       </c>
@@ -4199,7 +4210,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>90</v>
       </c>
@@ -4210,7 +4221,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>92</v>
       </c>
@@ -4221,7 +4232,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>94</v>
       </c>
@@ -4232,7 +4243,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>96</v>
       </c>
@@ -4243,7 +4254,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>98</v>
       </c>
@@ -4254,7 +4265,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>100</v>
       </c>
@@ -4265,7 +4276,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>102</v>
       </c>
@@ -4276,7 +4287,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>104</v>
       </c>
@@ -4287,7 +4298,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>106</v>
       </c>
@@ -4298,7 +4309,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>108</v>
       </c>
@@ -4309,7 +4320,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>110</v>
       </c>
@@ -4320,7 +4331,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>112</v>
       </c>
@@ -4331,7 +4342,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>114</v>
       </c>
@@ -4342,7 +4353,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>116</v>
       </c>
@@ -4353,7 +4364,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>118</v>
       </c>
@@ -4364,7 +4375,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>120</v>
       </c>
@@ -4375,7 +4386,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>122</v>
       </c>
@@ -4386,7 +4397,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>124</v>
       </c>
@@ -4397,7 +4408,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>126</v>
       </c>
@@ -4408,7 +4419,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>128</v>
       </c>
@@ -4419,7 +4430,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>130</v>
       </c>
@@ -4430,7 +4441,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>132</v>
       </c>
@@ -4441,7 +4452,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>134</v>
       </c>
@@ -4452,7 +4463,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>136</v>
       </c>
@@ -4463,7 +4474,7 @@
         <v>1048576</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>138</v>
       </c>
@@ -4474,7 +4485,7 @@
         <v>3072</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>140</v>
       </c>
@@ -4485,7 +4496,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>142</v>
       </c>
@@ -4496,7 +4507,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>144</v>
       </c>
@@ -4507,7 +4518,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>146</v>
       </c>
@@ -4518,7 +4529,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>148</v>
       </c>
@@ -4529,7 +4540,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>150</v>
       </c>
@@ -4540,7 +4551,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>152</v>
       </c>
@@ -4551,7 +4562,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>154</v>
       </c>
@@ -4562,7 +4573,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>156</v>
       </c>
@@ -4573,7 +4584,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>158</v>
       </c>
@@ -4584,7 +4595,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>160</v>
       </c>
@@ -4595,7 +4606,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>162</v>
       </c>
@@ -4606,7 +4617,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>164</v>
       </c>
@@ -4617,7 +4628,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>166</v>
       </c>
@@ -4628,7 +4639,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>168</v>
       </c>
@@ -4639,7 +4650,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>170</v>
       </c>
@@ -4650,7 +4661,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>172</v>
       </c>
@@ -4661,7 +4672,7 @@
         <v>59392</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>174</v>
       </c>
@@ -4672,7 +4683,7 @@
         <v>19456</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>176</v>
       </c>
@@ -4683,7 +4694,7 @@
         <v>12288</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>178</v>
       </c>
@@ -4694,7 +4705,7 @@
         <v>32768</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>180</v>
       </c>
@@ -4705,7 +4716,7 @@
         <v>57344</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>182</v>
       </c>
@@ -4716,7 +4727,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>184</v>
       </c>
@@ -4727,7 +4738,7 @@
         <v>73728</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>186</v>
       </c>
@@ -4738,7 +4749,7 @@
         <v>28672</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>188</v>
       </c>
@@ -4749,7 +4760,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>190</v>
       </c>
@@ -4760,7 +4771,7 @@
         <v>32768</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>192</v>
       </c>
@@ -4771,7 +4782,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>194</v>
       </c>
@@ -4782,7 +4793,7 @@
         <v>32768</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>196</v>
       </c>
@@ -4793,7 +4804,7 @@
         <v>6144</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>198</v>
       </c>
@@ -4804,7 +4815,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>200</v>
       </c>
@@ -4815,7 +4826,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>202</v>
       </c>
@@ -4826,7 +4837,7 @@
         <v>6912</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>204</v>
       </c>
@@ -4837,7 +4848,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>206</v>
       </c>
@@ -4848,7 +4859,7 @@
         <v>32768</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>208</v>
       </c>
@@ -4859,7 +4870,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>210</v>
       </c>
@@ -4870,7 +4881,7 @@
         <v>1536</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>212</v>
       </c>
@@ -4881,7 +4892,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>214</v>
       </c>
@@ -4892,7 +4903,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>216</v>
       </c>
@@ -4903,7 +4914,7 @@
         <v>1536</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>218</v>
       </c>
@@ -4914,7 +4925,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>220</v>
       </c>
@@ -4925,7 +4936,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>222</v>
       </c>
@@ -4936,7 +4947,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>224</v>
       </c>
@@ -4947,7 +4958,7 @@
         <v>20480</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>226</v>
       </c>
@@ -4958,7 +4969,7 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>228</v>
       </c>
@@ -4969,7 +4980,7 @@
         <v>12288</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>230</v>
       </c>
@@ -4980,7 +4991,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>232</v>
       </c>
@@ -4991,7 +5002,7 @@
         <v>12288</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>234</v>
       </c>
@@ -5002,7 +5013,7 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>236</v>
       </c>
@@ -5013,7 +5024,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>238</v>
       </c>
@@ -5024,7 +5035,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>240</v>
       </c>
@@ -5035,7 +5046,7 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>242</v>
       </c>
@@ -5046,7 +5057,7 @@
         <v>10240</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>244</v>
       </c>
@@ -5057,7 +5068,7 @@
         <v>26624</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>246</v>
       </c>
@@ -5068,7 +5079,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>248</v>
       </c>
@@ -5079,7 +5090,7 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>250</v>
       </c>
@@ -5090,7 +5101,7 @@
         <v>2560</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>252</v>
       </c>
@@ -5101,7 +5112,7 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>254</v>
       </c>
@@ -5112,7 +5123,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>256</v>
       </c>
@@ -5123,7 +5134,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>258</v>
       </c>
@@ -5134,7 +5145,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>260</v>
       </c>
@@ -5145,7 +5156,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>262</v>
       </c>
@@ -5156,7 +5167,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>264</v>
       </c>
@@ -5167,7 +5178,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>266</v>
       </c>
@@ -5178,7 +5189,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>268</v>
       </c>
@@ -5189,7 +5200,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>270</v>
       </c>
@@ -5200,7 +5211,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>272</v>
       </c>
@@ -5211,7 +5222,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>274</v>
       </c>
@@ -5222,7 +5233,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>276</v>
       </c>
@@ -5233,7 +5244,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>278</v>
       </c>
@@ -5244,7 +5255,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>280</v>
       </c>
@@ -5255,7 +5266,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>282</v>
       </c>
@@ -5266,7 +5277,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>284</v>
       </c>
@@ -5277,7 +5288,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>286</v>
       </c>
@@ -5288,7 +5299,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>288</v>
       </c>
@@ -5299,7 +5310,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>290</v>
       </c>
@@ -5310,7 +5321,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>292</v>
       </c>
@@ -5321,7 +5332,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>294</v>
       </c>
@@ -5332,7 +5343,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>296</v>
       </c>
@@ -5343,7 +5354,7 @@
         <v>32768</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>298</v>
       </c>
@@ -5354,7 +5365,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>300</v>
       </c>
@@ -5365,7 +5376,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>302</v>
       </c>
@@ -5376,7 +5387,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>304</v>
       </c>
@@ -5387,7 +5398,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>306</v>
       </c>
@@ -5398,7 +5409,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>308</v>
       </c>
@@ -5409,7 +5420,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>310</v>
       </c>
@@ -5420,7 +5431,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>312</v>
       </c>
@@ -5431,7 +5442,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>314</v>
       </c>
@@ -5442,7 +5453,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>316</v>
       </c>
@@ -5453,7 +5464,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>318</v>
       </c>
@@ -5464,7 +5475,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>320</v>
       </c>
@@ -5475,7 +5486,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>322</v>
       </c>
@@ -5486,7 +5497,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>324</v>
       </c>
@@ -5497,7 +5508,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>326</v>
       </c>
@@ -5508,7 +5519,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>328</v>
       </c>
@@ -5519,7 +5530,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>330</v>
       </c>
@@ -5530,7 +5541,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>332</v>
       </c>
@@ -5541,7 +5552,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>334</v>
       </c>
@@ -5552,7 +5563,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>336</v>
       </c>
@@ -5563,7 +5574,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>338</v>
       </c>
@@ -5574,7 +5585,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>340</v>
       </c>
@@ -5585,7 +5596,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>342</v>
       </c>
@@ -5596,7 +5607,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>344</v>
       </c>
@@ -5607,7 +5618,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>346</v>
       </c>
@@ -5618,7 +5629,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>348</v>
       </c>
@@ -5629,7 +5640,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>350</v>
       </c>
@@ -5640,7 +5651,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>352</v>
       </c>
@@ -5651,7 +5662,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>354</v>
       </c>
@@ -5662,7 +5673,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>356</v>
       </c>
@@ -5673,7 +5684,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>358</v>
       </c>
@@ -5684,7 +5695,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>360</v>
       </c>
@@ -5695,7 +5706,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>362</v>
       </c>
@@ -5706,7 +5717,7 @@
         <v>524288</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>364</v>
       </c>
@@ -5717,7 +5728,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>366</v>
       </c>
@@ -5728,7 +5739,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>368</v>
       </c>
@@ -5739,7 +5750,7 @@
         <v>148480</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>370</v>
       </c>
@@ -5750,7 +5761,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>372</v>
       </c>
@@ -5761,7 +5772,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>374</v>
       </c>
@@ -5772,7 +5783,7 @@
         <v>5120</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>376</v>
       </c>
@@ -5783,7 +5794,7 @@
         <v>59904</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>378</v>
       </c>
@@ -5794,7 +5805,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>380</v>
       </c>
@@ -5805,7 +5816,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>382</v>
       </c>
@@ -5816,7 +5827,7 @@
         <v>2560</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>384</v>
       </c>
@@ -5827,7 +5838,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>386</v>
       </c>
@@ -5838,7 +5849,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>388</v>
       </c>
@@ -5849,7 +5860,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>390</v>
       </c>
@@ -5860,7 +5871,7 @@
         <v>32768</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>392</v>
       </c>
@@ -5871,7 +5882,7 @@
         <v>7168</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>394</v>
       </c>
@@ -5882,7 +5893,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>396</v>
       </c>
@@ -5893,7 +5904,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>398</v>
       </c>
@@ -5904,7 +5915,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>400</v>
       </c>
@@ -5915,7 +5926,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>402</v>
       </c>
@@ -5926,7 +5937,7 @@
         <v>20480</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>404</v>
       </c>
@@ -5937,7 +5948,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>406</v>
       </c>
@@ -5948,7 +5959,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>408</v>
       </c>
@@ -5959,7 +5970,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>410</v>
       </c>
@@ -5970,7 +5981,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>412</v>
       </c>
@@ -5981,7 +5992,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>414</v>
       </c>
@@ -5992,7 +6003,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>416</v>
       </c>
@@ -6003,7 +6014,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>418</v>
       </c>
@@ -6014,7 +6025,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>420</v>
       </c>
@@ -6025,7 +6036,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
         <v>422</v>
       </c>
@@ -6036,7 +6047,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>424</v>
       </c>
@@ -6047,7 +6058,7 @@
         <v>55296</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>426</v>
       </c>
@@ -6058,7 +6069,7 @@
         <v>1792</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>428</v>
       </c>
@@ -6069,7 +6080,7 @@
         <v>7936</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>430</v>
       </c>
@@ -6080,7 +6091,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>432</v>
       </c>
@@ -6091,7 +6102,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>434</v>
       </c>
@@ -6102,7 +6113,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>436</v>
       </c>
@@ -6113,7 +6124,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>438</v>
       </c>
@@ -6124,7 +6135,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>440</v>
       </c>
@@ -6135,7 +6146,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>442</v>
       </c>
@@ -6146,7 +6157,7 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>444</v>
       </c>
@@ -6157,7 +6168,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
         <v>446</v>
       </c>
@@ -6168,7 +6179,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>448</v>
       </c>
@@ -6179,7 +6190,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>450</v>
       </c>
@@ -6190,7 +6201,7 @@
         <v>8704</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>452</v>
       </c>
@@ -6201,7 +6212,7 @@
         <v>1792</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>454</v>
       </c>
@@ -6212,7 +6223,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>456</v>
       </c>
@@ -6223,7 +6234,7 @@
         <v>3328</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>458</v>
       </c>
@@ -6234,7 +6245,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>460</v>
       </c>
@@ -6245,7 +6256,7 @@
         <v>12288</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>462</v>
       </c>
@@ -6256,7 +6267,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>464</v>
       </c>
@@ -6267,7 +6278,7 @@
         <v>2304</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
         <v>466</v>
       </c>
@@ -6278,7 +6289,7 @@
         <v>5376</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>468</v>
       </c>
@@ -6289,7 +6300,7 @@
         <v>6400</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
         <v>470</v>
       </c>
@@ -6300,7 +6311,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>472</v>
       </c>
@@ -6311,7 +6322,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
         <v>474</v>
       </c>
@@ -6322,7 +6333,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>476</v>
       </c>
@@ -6333,7 +6344,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
         <v>478</v>
       </c>
@@ -6344,7 +6355,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>480</v>
       </c>
@@ -6355,7 +6366,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
         <v>482</v>
       </c>
@@ -6366,7 +6377,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>484</v>
       </c>
@@ -6377,7 +6388,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
         <v>486</v>
       </c>
@@ -6388,7 +6399,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>488</v>
       </c>
@@ -6399,7 +6410,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
         <v>490</v>
       </c>
@@ -6410,7 +6421,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>492</v>
       </c>
@@ -6421,7 +6432,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
         <v>494</v>
       </c>
@@ -6432,7 +6443,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>496</v>
       </c>
@@ -6443,7 +6454,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
         <v>498</v>
       </c>
@@ -6454,7 +6465,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>500</v>
       </c>
@@ -6465,7 +6476,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
         <v>502</v>
       </c>
@@ -6476,7 +6487,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>504</v>
       </c>
@@ -6487,7 +6498,7 @@
         <v>32768</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
         <v>506</v>
       </c>
@@ -6498,7 +6509,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>508</v>
       </c>
@@ -6509,7 +6520,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
         <v>510</v>
       </c>
@@ -6520,7 +6531,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>512</v>
       </c>
@@ -6531,7 +6542,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
         <v>514</v>
       </c>
@@ -6542,7 +6553,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>516</v>
       </c>
@@ -6553,7 +6564,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
         <v>518</v>
       </c>
@@ -6564,7 +6575,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>520</v>
       </c>
@@ -6575,7 +6586,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
         <v>522</v>
       </c>
@@ -6586,7 +6597,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>524</v>
       </c>
@@ -6597,7 +6608,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
         <v>526</v>
       </c>
@@ -6608,7 +6619,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>528</v>
       </c>
@@ -6619,7 +6630,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
         <v>530</v>
       </c>
@@ -6630,7 +6641,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>532</v>
       </c>
@@ -6641,7 +6652,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
         <v>534</v>
       </c>
@@ -6652,7 +6663,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>536</v>
       </c>
@@ -6663,7 +6674,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
         <v>538</v>
       </c>
@@ -6674,7 +6685,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>540</v>
       </c>
@@ -6685,7 +6696,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
         <v>542</v>
       </c>
@@ -6696,7 +6707,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
         <v>544</v>
       </c>
@@ -6707,7 +6718,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
         <v>546</v>
       </c>
@@ -6718,7 +6729,7 @@
         <v>39168</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>548</v>
       </c>
@@ -6729,7 +6740,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
         <v>550</v>
       </c>
@@ -6740,7 +6751,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>552</v>
       </c>
@@ -6751,7 +6762,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
         <v>554</v>
       </c>
@@ -6762,7 +6773,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
         <v>556</v>
       </c>
@@ -6773,7 +6784,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" s="2" t="s">
         <v>558</v>
       </c>
@@ -6784,7 +6795,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
         <v>560</v>
       </c>
@@ -6795,7 +6806,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
         <v>562</v>
       </c>
@@ -6806,7 +6817,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
         <v>564</v>
       </c>
@@ -6817,7 +6828,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" s="2" t="s">
         <v>566</v>
       </c>
@@ -6828,7 +6839,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
         <v>568</v>
       </c>
@@ -6839,7 +6850,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" s="2" t="s">
         <v>570</v>
       </c>
@@ -6850,7 +6861,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
         <v>572</v>
       </c>
@@ -6861,7 +6872,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
         <v>574</v>
       </c>
@@ -6872,7 +6883,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
         <v>576</v>
       </c>
@@ -6883,7 +6894,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
         <v>578</v>
       </c>
@@ -6894,7 +6905,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>580</v>
       </c>
@@ -6905,7 +6916,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
         <v>582</v>
       </c>
@@ -6916,7 +6927,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
         <v>584</v>
       </c>
@@ -6927,7 +6938,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
         <v>586</v>
       </c>
@@ -6938,7 +6949,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
         <v>588</v>
       </c>
@@ -6949,7 +6960,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
         <v>590</v>
       </c>
@@ -6960,7 +6971,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
         <v>592</v>
       </c>
@@ -6971,7 +6982,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
         <v>594</v>
       </c>
@@ -6982,7 +6993,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
         <v>596</v>
       </c>
@@ -6993,7 +7004,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" s="2" t="s">
         <v>598</v>
       </c>
@@ -7004,7 +7015,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
         <v>600</v>
       </c>
@@ -7015,7 +7026,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" s="2" t="s">
         <v>602</v>
       </c>
@@ -7026,7 +7037,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
         <v>604</v>
       </c>
@@ -7037,7 +7048,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
         <v>606</v>
       </c>
@@ -7048,7 +7059,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
         <v>608</v>
       </c>
@@ -7059,7 +7070,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A307" s="2" t="s">
         <v>610</v>
       </c>
@@ -7070,7 +7081,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
         <v>612</v>
       </c>
@@ -7081,7 +7092,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A309" s="2" t="s">
         <v>614</v>
       </c>
@@ -7092,7 +7103,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
         <v>616</v>
       </c>
@@ -7103,7 +7114,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A311" s="2" t="s">
         <v>618</v>
       </c>
@@ -7114,7 +7125,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
         <v>620</v>
       </c>
@@ -7125,7 +7136,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
         <v>622</v>
       </c>
@@ -7136,7 +7147,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
         <v>624</v>
       </c>
@@ -7147,7 +7158,7 @@
         <v>7680</v>
       </c>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A315" s="2" t="s">
         <v>626</v>
       </c>
@@ -7158,7 +7169,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
         <v>628</v>
       </c>
@@ -7169,7 +7180,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A317" s="2" t="s">
         <v>630</v>
       </c>
@@ -7180,7 +7191,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
         <v>632</v>
       </c>
@@ -7191,7 +7202,7 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A319" s="2" t="s">
         <v>634</v>
       </c>
@@ -7202,7 +7213,7 @@
         <v>3328</v>
       </c>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
         <v>636</v>
       </c>
@@ -7213,7 +7224,7 @@
         <v>2304</v>
       </c>
     </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A321" s="2" t="s">
         <v>638</v>
       </c>
@@ -7224,7 +7235,7 @@
         <v>3328</v>
       </c>
     </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
         <v>640</v>
       </c>
@@ -7235,7 +7246,7 @@
         <v>3072</v>
       </c>
     </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A323" s="2" t="s">
         <v>642</v>
       </c>
@@ -7246,7 +7257,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
         <v>644</v>
       </c>
@@ -7257,7 +7268,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
         <v>646</v>
       </c>
@@ -7268,7 +7279,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
         <v>648</v>
       </c>
@@ -7279,7 +7290,7 @@
         <v>1536</v>
       </c>
     </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A327" s="2" t="s">
         <v>650</v>
       </c>
@@ -7290,7 +7301,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
         <v>652</v>
       </c>
@@ -7301,7 +7312,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A329" s="2" t="s">
         <v>654</v>
       </c>
@@ -7312,7 +7323,7 @@
         <v>1536</v>
       </c>
     </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A330" s="1" t="s">
         <v>656</v>
       </c>
@@ -7323,7 +7334,7 @@
         <v>2304</v>
       </c>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A331" s="2" t="s">
         <v>658</v>
       </c>
@@ -7334,7 +7345,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
         <v>660</v>
       </c>
@@ -7345,7 +7356,7 @@
         <v>13568</v>
       </c>
     </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A333" s="2" t="s">
         <v>662</v>
       </c>
@@ -7356,7 +7367,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
         <v>664</v>
       </c>
@@ -7367,7 +7378,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A335" s="2" t="s">
         <v>666</v>
       </c>
@@ -7378,7 +7389,7 @@
         <v>3328</v>
       </c>
     </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
         <v>668</v>
       </c>
@@ -7389,7 +7400,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A337" s="2" t="s">
         <v>670</v>
       </c>
@@ -7400,7 +7411,7 @@
         <v>2560</v>
       </c>
     </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
         <v>672</v>
       </c>
@@ -7411,7 +7422,7 @@
         <v>9728</v>
       </c>
     </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A339" s="2" t="s">
         <v>674</v>
       </c>
@@ -7422,7 +7433,7 @@
         <v>10752</v>
       </c>
     </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
         <v>676</v>
       </c>
@@ -7433,7 +7444,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A341" s="2" t="s">
         <v>678</v>
       </c>
@@ -7444,7 +7455,7 @@
         <v>4864</v>
       </c>
     </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
         <v>680</v>
       </c>
@@ -7455,7 +7466,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A343" s="2" t="s">
         <v>682</v>
       </c>
@@ -7466,7 +7477,7 @@
         <v>4608</v>
       </c>
     </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
         <v>684</v>
       </c>
@@ -7477,7 +7488,7 @@
         <v>9728</v>
       </c>
     </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A345" s="2" t="s">
         <v>686</v>
       </c>
@@ -7488,7 +7499,7 @@
         <v>2816</v>
       </c>
     </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
         <v>688</v>
       </c>
@@ -7499,7 +7510,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A347" s="2" t="s">
         <v>690</v>
       </c>
@@ -7510,7 +7521,7 @@
         <v>4608</v>
       </c>
     </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
         <v>692</v>
       </c>
@@ -7521,7 +7532,7 @@
         <v>9216</v>
       </c>
     </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A349" s="2" t="s">
         <v>694</v>
       </c>
@@ -7532,7 +7543,7 @@
         <v>3328</v>
       </c>
     </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
         <v>696</v>
       </c>
@@ -7543,7 +7554,7 @@
         <v>20992</v>
       </c>
     </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A351" s="2" t="s">
         <v>698</v>
       </c>
@@ -7554,7 +7565,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A352" s="1" t="s">
         <v>700</v>
       </c>
@@ -7565,7 +7576,7 @@
         <v>3584</v>
       </c>
     </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A353" s="2" t="s">
         <v>702</v>
       </c>
@@ -7576,7 +7587,7 @@
         <v>3072</v>
       </c>
     </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
         <v>704</v>
       </c>
@@ -7587,7 +7598,7 @@
         <v>5888</v>
       </c>
     </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A355" s="2" t="s">
         <v>706</v>
       </c>
@@ -7598,7 +7609,7 @@
         <v>3584</v>
       </c>
     </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
         <v>708</v>
       </c>
@@ -7609,7 +7620,7 @@
         <v>10240</v>
       </c>
     </row>
-    <row r="357" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A357" s="2" t="s">
         <v>710</v>
       </c>
@@ -7620,7 +7631,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="358" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
         <v>712</v>
       </c>
@@ -7631,7 +7642,7 @@
         <v>3072</v>
       </c>
     </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A359" s="2" t="s">
         <v>714</v>
       </c>
@@ -7642,7 +7653,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="360" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
         <v>716</v>
       </c>
@@ -7653,7 +7664,7 @@
         <v>22528</v>
       </c>
     </row>
-    <row r="361" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A361" s="2" t="s">
         <v>718</v>
       </c>
@@ -7664,7 +7675,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="362" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
         <v>720</v>
       </c>
@@ -7675,7 +7686,7 @@
         <v>1792</v>
       </c>
     </row>
-    <row r="363" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="363" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A363" s="2" t="s">
         <v>722</v>
       </c>
@@ -7686,7 +7697,7 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="364" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="364" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
         <v>724</v>
       </c>
@@ -7697,7 +7708,7 @@
         <v>5888</v>
       </c>
     </row>
-    <row r="365" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="365" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A365" s="2" t="s">
         <v>726</v>
       </c>
@@ -7708,7 +7719,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="366" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="366" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A366" s="1" t="s">
         <v>728</v>
       </c>
@@ -7719,7 +7730,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="367" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="367" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A367" s="2" t="s">
         <v>730</v>
       </c>
@@ -7730,7 +7741,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="368" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A368" s="1" t="s">
         <v>732</v>
       </c>
@@ -7741,7 +7752,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="369" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="369" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A369" s="2" t="s">
         <v>734</v>
       </c>
@@ -7752,7 +7763,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="370" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="370" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A370" s="1" t="s">
         <v>736</v>
       </c>
@@ -7763,7 +7774,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="371" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="371" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A371" s="2" t="s">
         <v>738</v>
       </c>
@@ -7774,7 +7785,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="372" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="372" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A372" s="1" t="s">
         <v>740</v>
       </c>
@@ -7785,7 +7796,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="373" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="373" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A373" s="2" t="s">
         <v>742</v>
       </c>
@@ -7796,7 +7807,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="374" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="374" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
         <v>744</v>
       </c>
@@ -7807,7 +7818,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="375" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A375" s="2" t="s">
         <v>746</v>
       </c>
@@ -7818,7 +7829,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="376" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="376" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
         <v>748</v>
       </c>
@@ -7829,7 +7840,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="377" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="377" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A377" s="2" t="s">
         <v>750</v>
       </c>
@@ -7840,7 +7851,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="378" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="378" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A378" s="1" t="s">
         <v>752</v>
       </c>
@@ -7851,7 +7862,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="379" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="379" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A379" s="2" t="s">
         <v>754</v>
       </c>
@@ -7862,7 +7873,7 @@
         <v>36608</v>
       </c>
     </row>
-    <row r="380" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="380" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
         <v>756</v>
       </c>
@@ -7873,7 +7884,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="381" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="381" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A381" s="2" t="s">
         <v>758</v>
       </c>
@@ -7884,7 +7895,7 @@
         <v>5376</v>
       </c>
     </row>
-    <row r="382" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="382" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A382" s="1" t="s">
         <v>760</v>
       </c>
@@ -7895,7 +7906,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="383" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="383" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A383" s="2" t="s">
         <v>762</v>
       </c>
@@ -7906,7 +7917,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="384" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="384" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A384" s="1" t="s">
         <v>764</v>
       </c>
@@ -7917,7 +7928,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="385" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="385" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A385" s="2" t="s">
         <v>766</v>
       </c>
@@ -7928,7 +7939,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="386" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="386" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A386" s="1" t="s">
         <v>768</v>
       </c>
@@ -7939,7 +7950,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="387" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="387" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A387" s="2" t="s">
         <v>770</v>
       </c>
@@ -7950,7 +7961,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="388" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="388" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A388" s="1" t="s">
         <v>772</v>
       </c>
@@ -7961,7 +7972,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="389" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="389" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A389" s="2" t="s">
         <v>774</v>
       </c>
@@ -7972,7 +7983,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="390" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="390" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A390" s="1" t="s">
         <v>776</v>
       </c>
@@ -7983,7 +7994,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="391" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="391" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A391" s="2" t="s">
         <v>778</v>
       </c>
@@ -7994,7 +8005,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="392" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="392" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A392" s="1" t="s">
         <v>780</v>
       </c>
@@ -8005,7 +8016,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="393" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="393" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A393" s="2" t="s">
         <v>782</v>
       </c>
@@ -8016,7 +8027,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="394" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="394" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A394" s="1" t="s">
         <v>784</v>
       </c>
@@ -8027,7 +8038,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="395" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="395" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A395" s="2" t="s">
         <v>786</v>
       </c>
@@ -8038,7 +8049,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="396" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="396" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A396" s="1" t="s">
         <v>788</v>
       </c>
@@ -8049,7 +8060,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="397" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="397" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A397" s="2" t="s">
         <v>790</v>
       </c>
@@ -8060,7 +8071,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="398" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="398" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A398" s="1" t="s">
         <v>792</v>
       </c>
@@ -8071,7 +8082,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="399" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="399" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A399" s="2" t="s">
         <v>794</v>
       </c>
@@ -8082,7 +8093,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="400" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="400" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A400" s="1" t="s">
         <v>796</v>
       </c>
@@ -8093,7 +8104,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="401" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="401" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A401" s="2" t="s">
         <v>798</v>
       </c>
@@ -8104,7 +8115,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="402" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="402" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A402" s="1" t="s">
         <v>800</v>
       </c>
@@ -8115,7 +8126,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="403" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="403" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A403" s="2" t="s">
         <v>802</v>
       </c>
@@ -8126,7 +8137,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="404" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="404" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A404" s="1" t="s">
         <v>804</v>
       </c>
@@ -8137,7 +8148,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="405" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="405" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A405" s="2" t="s">
         <v>806</v>
       </c>
@@ -8148,7 +8159,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="406" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="406" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A406" s="1" t="s">
         <v>808</v>
       </c>
@@ -8159,7 +8170,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="407" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="407" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A407" s="2" t="s">
         <v>810</v>
       </c>
@@ -8170,7 +8181,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="408" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="408" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A408" s="1" t="s">
         <v>812</v>
       </c>
@@ -8181,7 +8192,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="409" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="409" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A409" s="2" t="s">
         <v>814</v>
       </c>
@@ -8192,7 +8203,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="410" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="410" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A410" s="1" t="s">
         <v>816</v>
       </c>
@@ -8203,7 +8214,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="411" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="411" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A411" s="2" t="s">
         <v>818</v>
       </c>
@@ -8214,7 +8225,7 @@
         <v>1536</v>
       </c>
     </row>
-    <row r="412" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="412" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A412" s="1" t="s">
         <v>820</v>
       </c>
@@ -8225,7 +8236,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="413" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="413" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A413" s="2" t="s">
         <v>822</v>
       </c>
@@ -8236,7 +8247,7 @@
         <v>98304</v>
       </c>
     </row>
-    <row r="414" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="414" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A414" s="1" t="s">
         <v>824</v>
       </c>
@@ -8247,7 +8258,7 @@
         <v>13056</v>
       </c>
     </row>
-    <row r="415" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="415" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A415" s="2" t="s">
         <v>826</v>
       </c>
@@ -8258,7 +8269,7 @@
         <v>3072</v>
       </c>
     </row>
-    <row r="416" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="416" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A416" s="1" t="s">
         <v>828</v>
       </c>
@@ -8269,7 +8280,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="417" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="417" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A417" s="2" t="s">
         <v>830</v>
       </c>
@@ -8280,7 +8291,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="418" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="418" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A418" s="1" t="s">
         <v>832</v>
       </c>
@@ -8291,7 +8302,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="419" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="419" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A419" s="2" t="s">
         <v>834</v>
       </c>
@@ -8302,7 +8313,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="420" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="420" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A420" s="1" t="s">
         <v>836</v>
       </c>
@@ -8313,7 +8324,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="421" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="421" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A421" s="2" t="s">
         <v>838</v>
       </c>
@@ -8324,7 +8335,7 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="422" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="422" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A422" s="1" t="s">
         <v>840</v>
       </c>
@@ -8335,7 +8346,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="423" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="423" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A423" s="2" t="s">
         <v>842</v>
       </c>
@@ -8346,7 +8357,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="424" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="424" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A424" s="1" t="s">
         <v>844</v>
       </c>
@@ -8357,7 +8368,7 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="425" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="425" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A425" s="2" t="s">
         <v>846</v>
       </c>
@@ -8368,7 +8379,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="426" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="426" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A426" s="1" t="s">
         <v>848</v>
       </c>
@@ -8379,7 +8390,7 @@
         <v>262144</v>
       </c>
     </row>
-    <row r="427" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="427" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A427" s="2" t="s">
         <v>850</v>
       </c>
@@ -8390,7 +8401,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="428" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="428" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A428" s="1" t="s">
         <v>852</v>
       </c>
@@ -8401,7 +8412,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="429" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="429" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A429" s="2" t="s">
         <v>854</v>
       </c>
@@ -8412,7 +8423,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="430" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="430" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A430" s="1" t="s">
         <v>856</v>
       </c>
@@ -8423,7 +8434,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="431" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="431" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A431" s="2" t="s">
         <v>858</v>
       </c>
@@ -8434,7 +8445,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="432" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="432" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A432" s="1" t="s">
         <v>860</v>
       </c>
@@ -8445,7 +8456,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="433" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="433" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A433" s="2" t="s">
         <v>862</v>
       </c>
@@ -8456,7 +8467,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="434" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="434" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A434" s="1" t="s">
         <v>864</v>
       </c>
@@ -8467,7 +8478,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="435" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="435" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A435" s="2" t="s">
         <v>866</v>
       </c>
@@ -8478,7 +8489,7 @@
         <v>65536</v>
       </c>
     </row>
-    <row r="436" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="436" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A436" s="1" t="s">
         <v>868</v>
       </c>
@@ -8489,7 +8500,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="437" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="437" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A437" s="2" t="s">
         <v>870</v>
       </c>
@@ -8500,7 +8511,7 @@
         <v>3840</v>
       </c>
     </row>
-    <row r="438" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="438" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A438" s="1" t="s">
         <v>872</v>
       </c>
@@ -8511,7 +8522,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="439" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="439" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A439" s="2" t="s">
         <v>874</v>
       </c>
@@ -8522,7 +8533,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="440" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="440" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A440" s="1" t="s">
         <v>876</v>
       </c>
@@ -8533,7 +8544,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="441" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="441" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A441" s="2" t="s">
         <v>878</v>
       </c>
@@ -8544,7 +8555,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="442" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="442" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A442" s="1" t="s">
         <v>880</v>
       </c>
@@ -8555,7 +8566,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="443" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="443" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A443" s="2" t="s">
         <v>882</v>
       </c>
@@ -8566,7 +8577,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="444" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="444" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A444" s="1" t="s">
         <v>884</v>
       </c>
@@ -8577,7 +8588,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="445" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="445" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A445" s="2" t="s">
         <v>886</v>
       </c>
@@ -8588,7 +8599,7 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="446" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="446" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A446" s="1" t="s">
         <v>888</v>
       </c>
@@ -8599,7 +8610,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="447" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="447" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A447" s="2" t="s">
         <v>890</v>
       </c>
@@ -8610,7 +8621,7 @@
         <v>11264</v>
       </c>
     </row>
-    <row r="448" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="448" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A448" s="1" t="s">
         <v>892</v>
       </c>
@@ -8621,7 +8632,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="449" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="449" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A449" s="2" t="s">
         <v>894</v>
       </c>
@@ -8632,7 +8643,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="450" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="450" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A450" s="1" t="s">
         <v>896</v>
       </c>
@@ -8643,7 +8654,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="451" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="451" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A451" s="2" t="s">
         <v>898</v>
       </c>
@@ -8654,7 +8665,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="452" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="452" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A452" s="1" t="s">
         <v>900</v>
       </c>
@@ -8665,7 +8676,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="453" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="453" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A453" s="2" t="s">
         <v>902</v>
       </c>
@@ -8676,7 +8687,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="454" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="454" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A454" s="1" t="s">
         <v>904</v>
       </c>
@@ -8687,7 +8698,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="455" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="455" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A455" s="2" t="s">
         <v>906</v>
       </c>
@@ -8698,7 +8709,7 @@
         <v>2560</v>
       </c>
     </row>
-    <row r="456" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="456" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A456" s="1" t="s">
         <v>908</v>
       </c>
@@ -8709,7 +8720,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="457" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="457" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A457" s="2" t="s">
         <v>910</v>
       </c>
@@ -8720,7 +8731,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="458" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="458" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A458" s="1" t="s">
         <v>912</v>
       </c>
@@ -8731,7 +8742,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="459" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="459" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A459" s="2" t="s">
         <v>914</v>
       </c>
@@ -8742,7 +8753,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="460" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="460" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A460" s="1" t="s">
         <v>916</v>
       </c>
@@ -8753,7 +8764,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="461" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="461" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A461" s="2" t="s">
         <v>918</v>
       </c>
@@ -8764,7 +8775,7 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="462" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="462" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A462" s="1" t="s">
         <v>920</v>
       </c>
@@ -8775,7 +8786,7 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="463" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="463" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A463" s="2" t="s">
         <v>922</v>
       </c>
@@ -8786,7 +8797,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="464" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="464" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A464" s="1" t="s">
         <v>924</v>
       </c>
@@ -8797,7 +8808,7 @@
         <v>32768</v>
       </c>
     </row>
-    <row r="465" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="465" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A465" s="2" t="s">
         <v>926</v>
       </c>
@@ -8808,7 +8819,7 @@
         <v>5120</v>
       </c>
     </row>
-    <row r="466" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="466" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A466" s="1" t="s">
         <v>928</v>
       </c>
@@ -8819,7 +8830,7 @@
         <v>10240</v>
       </c>
     </row>
-    <row r="467" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="467" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A467" s="2" t="s">
         <v>930</v>
       </c>
@@ -8830,7 +8841,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="468" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="468" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A468" s="1" t="s">
         <v>932</v>
       </c>
@@ -8841,7 +8852,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="469" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="469" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A469" s="2" t="s">
         <v>934</v>
       </c>
@@ -8852,7 +8863,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="470" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="470" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A470" s="1" t="s">
         <v>936</v>
       </c>
@@ -8863,7 +8874,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="471" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="471" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A471" s="2" t="s">
         <v>938</v>
       </c>
@@ -8874,7 +8885,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="472" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="472" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A472" s="1" t="s">
         <v>940</v>
       </c>
@@ -8885,7 +8896,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="473" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="473" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A473" s="2" t="s">
         <v>942</v>
       </c>
@@ -8896,7 +8907,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="474" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="474" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A474" s="1" t="s">
         <v>944</v>
       </c>
@@ -8907,7 +8918,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="475" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="475" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A475" s="2" t="s">
         <v>946</v>
       </c>
@@ -8918,7 +8929,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="476" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="476" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A476" s="1" t="s">
         <v>948</v>
       </c>
@@ -8929,7 +8940,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="477" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="477" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A477" s="2" t="s">
         <v>950</v>
       </c>
@@ -8940,7 +8951,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="478" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="478" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A478" s="1" t="s">
         <v>952</v>
       </c>
@@ -8951,7 +8962,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="479" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="479" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A479" s="2" t="s">
         <v>954</v>
       </c>
@@ -8962,7 +8973,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="480" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="480" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A480" s="1" t="s">
         <v>956</v>
       </c>
@@ -8973,7 +8984,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="481" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="481" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A481" s="2" t="s">
         <v>958</v>
       </c>
@@ -8984,7 +8995,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="482" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="482" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A482" s="1" t="s">
         <v>960</v>
       </c>
@@ -8995,7 +9006,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="483" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="483" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A483" s="2" t="s">
         <v>962</v>
       </c>
@@ -9006,7 +9017,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="484" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="484" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A484" s="1" t="s">
         <v>964</v>
       </c>
@@ -9017,7 +9028,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="485" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="485" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A485" s="2" t="s">
         <v>966</v>
       </c>
@@ -9028,7 +9039,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="486" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="486" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A486" s="1" t="s">
         <v>968</v>
       </c>
@@ -9039,7 +9050,7 @@
         <v>32768</v>
       </c>
     </row>
-    <row r="487" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="487" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A487" s="2" t="s">
         <v>970</v>
       </c>
@@ -9050,7 +9061,7 @@
         <v>1792</v>
       </c>
     </row>
-    <row r="488" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="488" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A488" s="1" t="s">
         <v>972</v>
       </c>
@@ -9061,7 +9072,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="489" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="489" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A489" s="2" t="s">
         <v>974</v>
       </c>
@@ -9072,7 +9083,7 @@
         <v>2816</v>
       </c>
     </row>
-    <row r="490" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="490" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A490" s="1" t="s">
         <v>976</v>
       </c>
@@ -9083,7 +9094,7 @@
         <v>12800</v>
       </c>
     </row>
-    <row r="491" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="491" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A491" s="2" t="s">
         <v>978</v>
       </c>
@@ -9094,7 +9105,7 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="492" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="492" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A492" s="1" t="s">
         <v>980</v>
       </c>
@@ -9105,7 +9116,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="493" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="493" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A493" s="2" t="s">
         <v>982</v>
       </c>
@@ -9116,7 +9127,7 @@
         <v>24576</v>
       </c>
     </row>
-    <row r="494" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="494" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A494" s="1" t="s">
         <v>984</v>
       </c>
@@ -9127,7 +9138,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="495" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="495" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A495" s="2" t="s">
         <v>986</v>
       </c>
@@ -9138,7 +9149,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="496" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="496" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A496" s="1" t="s">
         <v>988</v>
       </c>
@@ -9149,7 +9160,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="497" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="497" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A497" s="2" t="s">
         <v>990</v>
       </c>
@@ -9160,7 +9171,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="498" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="498" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A498" s="1" t="s">
         <v>992</v>
       </c>
@@ -9171,7 +9182,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="499" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="499" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A499" s="2" t="s">
         <v>994</v>
       </c>
@@ -9182,7 +9193,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="500" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="500" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A500" s="1" t="s">
         <v>996</v>
       </c>
@@ -9193,7 +9204,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="501" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="501" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A501" s="2" t="s">
         <v>998</v>
       </c>
@@ -9204,7 +9215,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="502" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="502" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A502" s="1" t="s">
         <v>1000</v>
       </c>
@@ -9215,7 +9226,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="503" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="503" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A503" s="2" t="s">
         <v>1002</v>
       </c>
@@ -9226,7 +9237,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="504" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="504" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A504" s="1" t="s">
         <v>1004</v>
       </c>
@@ -9237,7 +9248,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="505" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="505" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A505" s="2" t="s">
         <v>1006</v>
       </c>
@@ -9248,7 +9259,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="506" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="506" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A506" s="1" t="s">
         <v>1008</v>
       </c>
@@ -9259,7 +9270,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="507" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="507" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A507" s="2" t="s">
         <v>1010</v>
       </c>
@@ -9270,7 +9281,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="508" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="508" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A508" s="1" t="s">
         <v>1012</v>
       </c>
@@ -9281,7 +9292,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="509" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="509" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A509" s="2" t="s">
         <v>1014</v>
       </c>
@@ -9292,7 +9303,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="510" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="510" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A510" s="1" t="s">
         <v>1016</v>
       </c>
@@ -9303,7 +9314,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="511" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="511" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A511" s="2" t="s">
         <v>1018</v>
       </c>
@@ -9314,7 +9325,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="512" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="512" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A512" s="1" t="s">
         <v>1020</v>
       </c>
@@ -9325,7 +9336,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="513" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="513" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A513" s="2" t="s">
         <v>1022</v>
       </c>
@@ -9336,7 +9347,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="514" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="514" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A514" s="1" t="s">
         <v>1024</v>
       </c>
@@ -9347,7 +9358,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="515" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="515" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A515" s="2" t="s">
         <v>1026</v>
       </c>
@@ -9358,7 +9369,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="516" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="516" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A516" s="1" t="s">
         <v>1028</v>
       </c>
@@ -9369,7 +9380,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="517" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="517" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A517" s="2" t="s">
         <v>1030</v>
       </c>
@@ -9380,7 +9391,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="518" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="518" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A518" s="1" t="s">
         <v>1032</v>
       </c>
@@ -9391,7 +9402,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="519" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="519" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A519" s="2" t="s">
         <v>1034</v>
       </c>
@@ -9402,7 +9413,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="520" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="520" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A520" s="1" t="s">
         <v>1036</v>
       </c>
@@ -9413,7 +9424,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="521" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="521" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A521" s="2" t="s">
         <v>1038</v>
       </c>
@@ -9424,7 +9435,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="522" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="522" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A522" s="1" t="s">
         <v>1040</v>
       </c>
@@ -9435,7 +9446,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="523" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="523" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A523" s="2" t="s">
         <v>1042</v>
       </c>
@@ -9446,7 +9457,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="524" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="524" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A524" s="1" t="s">
         <v>1044</v>
       </c>
@@ -9457,7 +9468,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="525" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="525" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A525" s="2" t="s">
         <v>1046</v>
       </c>
@@ -9468,7 +9479,7 @@
         <v>4608</v>
       </c>
     </row>
-    <row r="526" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="526" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A526" s="1" t="s">
         <v>1048</v>
       </c>
@@ -9479,7 +9490,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="527" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="527" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A527" s="2" t="s">
         <v>1050</v>
       </c>
@@ -9490,7 +9501,7 @@
         <v>65536</v>
       </c>
     </row>
-    <row r="528" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="528" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A528" s="1" t="s">
         <v>1052</v>
       </c>
@@ -9501,7 +9512,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="529" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="529" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A529" s="2" t="s">
         <v>1054</v>
       </c>
@@ -9512,7 +9523,7 @@
         <v>5120</v>
       </c>
     </row>
-    <row r="530" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="530" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A530" s="1" t="s">
         <v>1056</v>
       </c>
@@ -9523,7 +9534,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="531" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="531" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A531" s="2" t="s">
         <v>1058</v>
       </c>
@@ -9534,7 +9545,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="532" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="532" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A532" s="1" t="s">
         <v>1060</v>
       </c>
@@ -9545,7 +9556,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="533" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="533" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A533" s="2" t="s">
         <v>1062</v>
       </c>
@@ -9556,7 +9567,7 @@
         <v>5888</v>
       </c>
     </row>
-    <row r="534" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="534" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A534" s="1" t="s">
         <v>1064</v>
       </c>
@@ -9567,7 +9578,7 @@
         <v>32768</v>
       </c>
     </row>
-    <row r="535" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="535" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A535" s="2" t="s">
         <v>1066</v>
       </c>
@@ -9578,7 +9589,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="536" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="536" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A536" s="1" t="s">
         <v>1068</v>
       </c>
@@ -9589,7 +9600,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="537" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="537" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A537" s="2" t="s">
         <v>1070</v>
       </c>
@@ -9600,7 +9611,7 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="538" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="538" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A538" s="1" t="s">
         <v>1072</v>
       </c>
@@ -9611,7 +9622,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="539" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="539" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A539" s="2" t="s">
         <v>1074</v>
       </c>
@@ -9622,7 +9633,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="540" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="540" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A540" s="1" t="s">
         <v>1076</v>
       </c>
@@ -9633,7 +9644,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="541" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="541" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A541" s="2" t="s">
         <v>1078</v>
       </c>
@@ -9644,7 +9655,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="542" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="542" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A542" s="1" t="s">
         <v>1080</v>
       </c>
@@ -9655,7 +9666,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="543" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="543" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A543" s="2" t="s">
         <v>1082</v>
       </c>

</xml_diff>

<commit_message>
adding the files needed to check the IPs
</commit_message>
<xml_diff>
--- a/files/rangeOfIPAddresses.xlsx
+++ b/files/rangeOfIPAddresses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atish\Desktop\Programming\TLDR Fail\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6007B6B-B080-4B7B-A9A3-DE2096123A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5654FD05-BC72-4E9A-A1C3-4E8C959B3077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{EECDF66F-84CF-47E0-9AA0-E9C9E9760CBF}"/>
+    <workbookView minimized="1" xWindow="3030" yWindow="3030" windowWidth="15375" windowHeight="8325" xr2:uid="{EECDF66F-84CF-47E0-9AA0-E9C9E9760CBF}"/>
   </bookViews>
   <sheets>
     <sheet name="ipAddresses" sheetId="1" r:id="rId1"/>
@@ -3687,8 +3687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0677CDAD-B304-45E8-80F1-C56675B70DA3}">
   <dimension ref="A1:D543"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="310" zoomScaleNormal="310" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" zoomScale="295" zoomScaleNormal="295" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>